<commit_message>
trying to get dummies with a loop
</commit_message>
<xml_diff>
--- a/attributes.xlsx
+++ b/attributes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kas\Documents\Feature-Engineering-8\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECC21239-4E51-4CC9-9934-8ADFE3C0704F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="14235" windowHeight="12735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="train" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
   <si>
     <t>Id</t>
   </si>
@@ -268,9 +274,6 @@
     <t>dummies</t>
   </si>
   <si>
-    <t>Talk more</t>
-  </si>
-  <si>
     <t>talk more about this and the below</t>
   </si>
   <si>
@@ -284,13 +287,16 @@
   </si>
   <si>
     <t>Response</t>
+  </si>
+  <si>
+    <t>categorical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -907,6 +913,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -953,7 +967,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -985,9 +999,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1019,6 +1051,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1194,37 +1244,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="42" max="42" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1235,7 +1285,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1246,23 +1296,23 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1270,7 +1320,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1278,15 +1328,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1294,7 +1344,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1302,7 +1352,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1310,7 +1360,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1318,15 +1368,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1334,7 +1384,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1342,7 +1392,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1350,7 +1400,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1358,7 +1408,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1366,10 +1416,10 @@
         <v>82</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1377,378 +1427,440 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="B23" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="B24" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="B25" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="B26" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="B27" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="B29" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="B30" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="B31" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="B32" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="5"/>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="B33" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="B34" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="5"/>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="B35" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="B37" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="5"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="5"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="5"/>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="5"/>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="B41" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="5"/>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="B42" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="5"/>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="B43" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="5"/>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="B44" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="5"/>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="5"/>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="5"/>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="5"/>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B49" s="5"/>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B50" s="5"/>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="5"/>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="5"/>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B53" s="5"/>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B54" s="5"/>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="5"/>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="B55" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B56" s="5"/>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="5"/>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="B57" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B58" s="5"/>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="5"/>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="B59" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="5"/>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="B60" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B61" s="5"/>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="5"/>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="B62" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B63" s="5"/>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B64" s="5"/>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="5"/>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="B65" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="5"/>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="B66" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B67" s="5"/>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="B67" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B68" s="5"/>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B69" s="5"/>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="5"/>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B71" s="5"/>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B72" s="5"/>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="5"/>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="5"/>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="B74" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B75" s="5"/>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="B75" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B76" s="5"/>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="B76" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B77" s="5"/>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="B77" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B78" s="5"/>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B79" s="5"/>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B80" s="5"/>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="B80" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B81" s="5"/>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="B81" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>80</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>